<commit_message>
add WIFI MODULE AP6275P
</commit_message>
<xml_diff>
--- a/WyyComponentDatabase.xlsx
+++ b/WyyComponentDatabase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cadence\SPB_Data\Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50060497-AEED-477C-8F45-8FFAFBD5D322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281734DF-9ECD-4AC7-BF20-8B99CD1915E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="贴片电阻" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2865" uniqueCount="1592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2873" uniqueCount="1599">
   <si>
     <t>Part Number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6199,6 +6199,34 @@
   </si>
   <si>
     <t>BORN(伯恩半导体)</t>
+  </si>
+  <si>
+    <t>WIFI模块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7001100003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wi-Fi and Bluetooth  module;802.11a/b/g/n/ac/ax 2x2 MIMO 1200Mbps;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>正基</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AP6275PR3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>md50_wifi-ap6275p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AP6275P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -12797,10 +12825,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F61549-8124-4EE7-A218-E5BC471FD40D}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -12808,7 +12836,7 @@
     <col min="1" max="1" width="12.25" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.875" bestFit="1" customWidth="1"/>
@@ -12922,6 +12950,32 @@
       </c>
       <c r="I4" t="s">
         <v>1532</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1592</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1598</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1594</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1595</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1596</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1597</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1598</v>
       </c>
     </row>
   </sheetData>
@@ -15480,9 +15534,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F28B83C-EC15-4DE5-B23D-95C2173BD368}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add MT7968a mt7976g mt7976a
</commit_message>
<xml_diff>
--- a/WyyComponentDatabase.xlsx
+++ b/WyyComponentDatabase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cadence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBD4FC7-85C2-4144-9638-D52262EBD6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610F69C9-AE57-4A1A-BFB1-D8B7724D7E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="贴片电阻" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <sheet name="其他芯片" sheetId="11" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">电源IC!$A$1:$J$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">电源IC!$A$1:$J$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">晶体管!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">其他芯片!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">贴片电容!$A$1:$J$1</definedName>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3078" uniqueCount="1724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3134" uniqueCount="1755">
   <si>
     <t>Part Number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6719,6 +6719,128 @@
   </si>
   <si>
     <t>IND POWER Coil;3.3uH;+/-20%;DRC=38mΩ;5.5A;5.2*5.4*2.8mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1111665200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>66.5K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RES FILM;66.5KΩ;+/-1%;1/16W;0402</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RC0402FR-0766K5L</t>
+  </si>
+  <si>
+    <t>39R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RES FILM;39Ω;+/-1%;1/16W;0402</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1111390001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RC0402FR-0739RL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CXDQ3BFAM-IJ-A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDRAM-DDR4 8Gb 3200Mb/s 1.2V 并口 96-FBGA(7.5x13mm)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CXMT(长鑫存储)</t>
+  </si>
+  <si>
+    <t>1511300009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英飞凌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TDA21472</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2051000012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MT7986A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WIFI芯片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2051000013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2051000014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MediaTek</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MT7986A_BGA_37</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MT7976G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MT7662E-20121128_51</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MT7662E-20121128_52</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MT7976A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MT7976GN is an IEEE WiFi 6 MIMO RF chip which contains 2.4 GHz WI-Fi transceiver front-ends in a DRQFN package;DRQFN144</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MT7976AN is an IEEE WiFi 6 MIMO RF chip which contains 5 GHz WI-Fi transceiver front-ends in a DRQFN package;DRQFN144</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quad-core ARM® Cortex-A53;Two HSGMII(2.5Gbps) interfaces;Lead in 4x4+4x4 WIFI6E integration;HW QoS;HW NAT;VFBGA57</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VFBGA57</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RQFN144</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMS1117</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6729,7 +6851,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6766,6 +6888,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF4E4E4E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -6787,7 +6915,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -6800,6 +6928,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -7080,11 +7209,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J119"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I64" sqref="I64"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8816,25 +8945,25 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>1530</v>
+        <v>1730</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1529</v>
+        <v>1728</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1531</v>
+        <v>1729</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>1528</v>
+        <v>1731</v>
       </c>
       <c r="G67" t="s">
-        <v>332</v>
+        <v>19</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>339</v>
@@ -8842,25 +8971,25 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>130</v>
+        <v>1530</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>272</v>
+        <v>1529</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>834</v>
+        <v>1531</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>701</v>
+        <v>1528</v>
       </c>
       <c r="G68" t="s">
-        <v>19</v>
+        <v>332</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>339</v>
@@ -8868,7 +8997,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>699</v>
+        <v>130</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>10</v>
@@ -8877,16 +9006,16 @@
         <v>272</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="G69" t="s">
-        <v>332</v>
+        <v>19</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>339</v>
@@ -8894,25 +9023,25 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>1078</v>
+        <v>699</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1079</v>
+        <v>272</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>1173</v>
+        <v>835</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>1080</v>
+        <v>700</v>
       </c>
       <c r="G70" t="s">
-        <v>19</v>
+        <v>332</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>339</v>
@@ -8920,22 +9049,22 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>1535</v>
+        <v>1078</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1534</v>
+        <v>1079</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>1536</v>
+        <v>1173</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>1537</v>
+        <v>1080</v>
       </c>
       <c r="G71" t="s">
         <v>19</v>
@@ -8946,22 +9075,22 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>1172</v>
+        <v>1535</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1171</v>
+        <v>1534</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>1174</v>
+        <v>1536</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>1175</v>
+        <v>1537</v>
       </c>
       <c r="G72" t="s">
         <v>19</v>
@@ -8972,22 +9101,22 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>1056</v>
+        <v>1172</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1052</v>
+        <v>1171</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1053</v>
+        <v>1174</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>1054</v>
+        <v>1175</v>
       </c>
       <c r="G73" t="s">
         <v>19</v>
@@ -8998,22 +9127,22 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>1551</v>
+        <v>1056</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1550</v>
+        <v>1052</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>1552</v>
+        <v>1053</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>1553</v>
+        <v>1054</v>
       </c>
       <c r="G74" t="s">
         <v>19</v>
@@ -9024,25 +9153,25 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>410</v>
+        <v>1551</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>406</v>
+        <v>1550</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>408</v>
+        <v>1552</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>412</v>
+        <v>1553</v>
       </c>
       <c r="G75" t="s">
-        <v>332</v>
+        <v>19</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>339</v>
@@ -9050,22 +9179,22 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>472</v>
+        <v>410</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>470</v>
+        <v>406</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>471</v>
+        <v>408</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>469</v>
+        <v>412</v>
       </c>
       <c r="G76" t="s">
         <v>332</v>
@@ -9076,7 +9205,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>10</v>
@@ -9085,16 +9214,16 @@
         <v>470</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>486</v>
+        <v>471</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>485</v>
+        <v>469</v>
       </c>
       <c r="G77" t="s">
-        <v>19</v>
+        <v>332</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>339</v>
@@ -9102,25 +9231,25 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>430</v>
+        <v>484</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>432</v>
+        <v>470</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>433</v>
+        <v>486</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>434</v>
+        <v>485</v>
       </c>
       <c r="G78" t="s">
-        <v>332</v>
+        <v>19</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>339</v>
@@ -9128,25 +9257,25 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>1089</v>
+        <v>430</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1090</v>
+        <v>432</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1091</v>
+        <v>433</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>1092</v>
+        <v>434</v>
       </c>
       <c r="G79" t="s">
-        <v>19</v>
+        <v>332</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>339</v>
@@ -9154,22 +9283,22 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>1448</v>
+        <v>1089</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1446</v>
+        <v>1090</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1449</v>
+        <v>1091</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>1447</v>
+        <v>1092</v>
       </c>
       <c r="G80" t="s">
         <v>19</v>
@@ -9180,22 +9309,22 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>163</v>
+        <v>1448</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>273</v>
+        <v>1446</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>133</v>
+        <v>1449</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>162</v>
+        <v>1447</v>
       </c>
       <c r="G81" t="s">
         <v>19</v>
@@ -9206,22 +9335,22 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>367</v>
+        <v>163</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>364</v>
+        <v>273</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>372</v>
+        <v>133</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>363</v>
+        <v>162</v>
       </c>
       <c r="G82" t="s">
         <v>19</v>
@@ -9232,7 +9361,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>10</v>
@@ -9241,16 +9370,16 @@
         <v>364</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>332</v>
+        <v>363</v>
+      </c>
+      <c r="G83" t="s">
+        <v>19</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>339</v>
@@ -9258,7 +9387,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>1098</v>
+        <v>368</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>10</v>
@@ -9267,16 +9396,16 @@
         <v>364</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1099</v>
+        <v>365</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1100</v>
-      </c>
-      <c r="G84" t="s">
-        <v>19</v>
+        <v>366</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>332</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>339</v>
@@ -9284,22 +9413,22 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>153</v>
+        <v>1098</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>274</v>
+        <v>364</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>154</v>
+        <v>1099</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>152</v>
+        <v>1100</v>
       </c>
       <c r="G85" t="s">
         <v>19</v>
@@ -9310,22 +9439,22 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G86" t="s">
         <v>19</v>
@@ -9336,7 +9465,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>452</v>
+        <v>157</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>10</v>
@@ -9345,16 +9474,16 @@
         <v>275</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>453</v>
+        <v>156</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>454</v>
+        <v>155</v>
       </c>
       <c r="G87" t="s">
-        <v>332</v>
+        <v>19</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>339</v>
@@ -9362,25 +9491,25 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>1032</v>
+        <v>452</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1031</v>
+        <v>275</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>1046</v>
+        <v>453</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>1033</v>
+        <v>454</v>
       </c>
       <c r="G88" t="s">
-        <v>19</v>
+        <v>332</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>339</v>
@@ -9388,7 +9517,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>1462</v>
+        <v>1032</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>10</v>
@@ -9397,16 +9526,16 @@
         <v>1031</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>1463</v>
+        <v>1046</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>1464</v>
+        <v>1033</v>
       </c>
       <c r="G89" t="s">
-        <v>332</v>
+        <v>19</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>339</v>
@@ -9414,25 +9543,25 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>1044</v>
+        <v>1462</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1043</v>
+        <v>1031</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1045</v>
+        <v>1463</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>1042</v>
+        <v>1464</v>
       </c>
       <c r="G90" t="s">
-        <v>19</v>
+        <v>332</v>
       </c>
       <c r="I90" s="1" t="s">
         <v>339</v>
@@ -9440,7 +9569,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>1465</v>
+        <v>1044</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>10</v>
@@ -9449,16 +9578,16 @@
         <v>1043</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>1466</v>
+        <v>1045</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1467</v>
+        <v>1042</v>
       </c>
       <c r="G91" t="s">
-        <v>332</v>
+        <v>19</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>339</v>
@@ -9466,22 +9595,22 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>946</v>
+        <v>1465</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>947</v>
+        <v>1043</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>948</v>
+        <v>1466</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>949</v>
+        <v>1467</v>
       </c>
       <c r="G92" t="s">
         <v>332</v>
@@ -9492,25 +9621,25 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>1295</v>
+        <v>946</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1296</v>
+        <v>947</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>1297</v>
+        <v>948</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>1599</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>19</v>
+        <v>949</v>
+      </c>
+      <c r="G93" t="s">
+        <v>332</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>339</v>
@@ -9518,24 +9647,24 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>1160</v>
+        <v>1295</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1159</v>
+        <v>1296</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>1162</v>
+        <v>1297</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>1161</v>
-      </c>
-      <c r="G94" t="s">
+        <v>1599</v>
+      </c>
+      <c r="G94" s="1" t="s">
         <v>19</v>
       </c>
       <c r="I94" s="1" t="s">
@@ -9544,22 +9673,22 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>1592</v>
+        <v>1160</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1593</v>
+        <v>1159</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>1594</v>
+        <v>1162</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>1595</v>
+        <v>1161</v>
       </c>
       <c r="G95" t="s">
         <v>19</v>
@@ -9570,22 +9699,22 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>1702</v>
+        <v>1592</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1703</v>
+        <v>1593</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1704</v>
+        <v>1594</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>1705</v>
+        <v>1595</v>
       </c>
       <c r="G96" t="s">
         <v>19</v>
@@ -9596,22 +9725,22 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>1484</v>
+        <v>1702</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1483</v>
+        <v>1703</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>1485</v>
+        <v>1704</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>1486</v>
+        <v>1705</v>
       </c>
       <c r="G97" t="s">
         <v>19</v>
@@ -9622,25 +9751,25 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>681</v>
+        <v>1484</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>680</v>
+        <v>1483</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>679</v>
+        <v>1485</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>678</v>
+        <v>1486</v>
       </c>
       <c r="G98" t="s">
-        <v>332</v>
+        <v>19</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>339</v>
@@ -9648,22 +9777,22 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>698</v>
+        <v>678</v>
       </c>
       <c r="G99" t="s">
         <v>332</v>
@@ -9674,25 +9803,25 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>608</v>
+        <v>689</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>609</v>
+        <v>688</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>610</v>
+        <v>687</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>611</v>
+        <v>698</v>
       </c>
       <c r="G100" t="s">
-        <v>19</v>
+        <v>332</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>339</v>
@@ -9700,25 +9829,25 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>402</v>
+        <v>608</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>401</v>
+        <v>609</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>404</v>
+        <v>610</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>403</v>
+        <v>611</v>
       </c>
       <c r="G101" t="s">
-        <v>332</v>
+        <v>19</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>339</v>
@@ -9726,24 +9855,24 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>331</v>
+        <v>402</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>330</v>
+        <v>401</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>329</v>
+        <v>404</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="G102" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="G102" t="s">
         <v>332</v>
       </c>
       <c r="I102" s="1" t="s">
@@ -9752,7 +9881,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>10</v>
@@ -9761,16 +9890,16 @@
         <v>330</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>1084</v>
-      </c>
-      <c r="G103" t="s">
-        <v>19</v>
+        <v>328</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>332</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>339</v>
@@ -9778,22 +9907,22 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>1156</v>
+        <v>338</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1155</v>
+        <v>330</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>1158</v>
+        <v>337</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>1157</v>
+        <v>1084</v>
       </c>
       <c r="G104" t="s">
         <v>19</v>
@@ -9804,22 +9933,22 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>1081</v>
+        <v>1156</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1082</v>
+        <v>1155</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1083</v>
+        <v>1158</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>1085</v>
+        <v>1157</v>
       </c>
       <c r="G105" t="s">
         <v>19</v>
@@ -9830,22 +9959,22 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>1696</v>
+        <v>1724</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1695</v>
+        <v>1725</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>1083</v>
+        <v>1726</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>1697</v>
+        <v>1727</v>
       </c>
       <c r="G106" t="s">
         <v>19</v>
@@ -9856,22 +9985,22 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>1280</v>
+        <v>1081</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1279</v>
+        <v>1082</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1281</v>
+        <v>1083</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>1282</v>
+        <v>1085</v>
       </c>
       <c r="G107" t="s">
         <v>19</v>
@@ -9882,22 +10011,22 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>1105</v>
+        <v>1696</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1106</v>
+        <v>1695</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>1107</v>
+        <v>1083</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>1108</v>
+        <v>1697</v>
       </c>
       <c r="G108" t="s">
         <v>19</v>
@@ -9908,22 +10037,22 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>830</v>
+        <v>1280</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>829</v>
+        <v>1279</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>831</v>
+        <v>1281</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>828</v>
+        <v>1282</v>
       </c>
       <c r="G109" t="s">
         <v>19</v>
@@ -9934,22 +10063,22 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>1311</v>
+        <v>1105</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1310</v>
+        <v>1106</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>1312</v>
+        <v>1107</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>1313</v>
+        <v>1108</v>
       </c>
       <c r="G110" t="s">
         <v>19</v>
@@ -9960,22 +10089,22 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>624</v>
+        <v>830</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>623</v>
+        <v>829</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>622</v>
+        <v>831</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>621</v>
+        <v>828</v>
       </c>
       <c r="G111" t="s">
         <v>19</v>
@@ -9986,22 +10115,22 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>1397</v>
+        <v>1311</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1396</v>
+        <v>1310</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>1398</v>
+        <v>1312</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>1399</v>
+        <v>1313</v>
       </c>
       <c r="G112" t="s">
         <v>19</v>
@@ -10012,22 +10141,22 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>134</v>
+        <v>624</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>271</v>
+        <v>623</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>133</v>
+        <v>622</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>131</v>
+        <v>621</v>
       </c>
       <c r="G113" t="s">
         <v>19</v>
@@ -10038,22 +10167,22 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>1547</v>
+        <v>1397</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1546</v>
+        <v>1396</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>1548</v>
+        <v>1398</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>1549</v>
+        <v>1399</v>
       </c>
       <c r="G114" t="s">
         <v>19</v>
@@ -10064,25 +10193,25 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>692</v>
+        <v>134</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>691</v>
+        <v>271</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>690</v>
+        <v>133</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>697</v>
+        <v>131</v>
       </c>
       <c r="G115" t="s">
-        <v>332</v>
+        <v>19</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>339</v>
@@ -10090,22 +10219,22 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>1055</v>
+        <v>1547</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1057</v>
+        <v>1546</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>1058</v>
+        <v>1548</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>1059</v>
+        <v>1549</v>
       </c>
       <c r="G116" t="s">
         <v>19</v>
@@ -10116,22 +10245,22 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>400</v>
+        <v>692</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>399</v>
+        <v>691</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>405</v>
+        <v>690</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>403</v>
+        <v>697</v>
       </c>
       <c r="G117" t="s">
         <v>332</v>
@@ -10142,25 +10271,25 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>696</v>
+        <v>1055</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>695</v>
+        <v>1057</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>694</v>
+        <v>1058</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>693</v>
+        <v>1059</v>
       </c>
       <c r="G118" t="s">
-        <v>332</v>
+        <v>19</v>
       </c>
       <c r="I118" s="1" t="s">
         <v>339</v>
@@ -10168,27 +10297,79 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="G119" t="s">
+        <v>332</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="G120" t="s">
+        <v>332</v>
+      </c>
+      <c r="I120" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
         <v>1670</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>1668</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C121" s="1" t="s">
         <v>1669</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>1671</v>
       </c>
-      <c r="E119" s="1" t="s">
+      <c r="E121" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F119" s="1" t="s">
+      <c r="F121" s="1" t="s">
         <v>1672</v>
       </c>
-      <c r="G119" s="1" t="s">
+      <c r="G121" s="1" t="s">
         <v>1673</v>
       </c>
-      <c r="I119" s="1" t="s">
+      <c r="I121" s="1" t="s">
         <v>1674</v>
       </c>
     </row>
@@ -10208,8 +10389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A56977-BF1C-4909-8B1B-32F3873FBB32}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10515,7 +10696,7 @@
         <v>979</v>
       </c>
       <c r="I11" t="s">
-        <v>980</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -10990,7 +11171,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J28" xr:uid="{47A56977-BF1C-4909-8B1B-32F3873FBB32}">
+  <autoFilter ref="A1:J29" xr:uid="{47A56977-BF1C-4909-8B1B-32F3873FBB32}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J28">
       <sortCondition ref="A1:A28"/>
     </sortState>
@@ -11663,10 +11844,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC4AD67-C776-4093-88E2-79BBC414D956}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11949,417 +12130,443 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>595</v>
+        <v>1523</v>
       </c>
       <c r="B11" t="s">
-        <v>594</v>
+        <v>383</v>
       </c>
       <c r="C11" t="s">
-        <v>596</v>
+        <v>1732</v>
       </c>
       <c r="D11" t="s">
-        <v>597</v>
-      </c>
-      <c r="E11" t="s">
-        <v>600</v>
+        <v>1733</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>1734</v>
       </c>
       <c r="F11" t="s">
-        <v>599</v>
+        <v>1732</v>
       </c>
       <c r="G11" t="s">
-        <v>598</v>
+        <v>1019</v>
       </c>
       <c r="I11" t="s">
-        <v>596</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>842</v>
+        <v>595</v>
       </c>
       <c r="B12" t="s">
         <v>594</v>
       </c>
       <c r="C12" t="s">
-        <v>843</v>
+        <v>596</v>
       </c>
       <c r="D12" t="s">
-        <v>844</v>
+        <v>597</v>
       </c>
       <c r="E12" t="s">
-        <v>846</v>
+        <v>600</v>
       </c>
       <c r="F12" t="s">
-        <v>847</v>
+        <v>599</v>
       </c>
       <c r="G12" t="s">
-        <v>845</v>
+        <v>598</v>
       </c>
       <c r="I12" t="s">
-        <v>843</v>
+        <v>596</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>1655</v>
+        <v>842</v>
       </c>
       <c r="B13" t="s">
-        <v>303</v>
+        <v>594</v>
       </c>
       <c r="C13" t="s">
-        <v>302</v>
+        <v>843</v>
       </c>
       <c r="D13" t="s">
-        <v>301</v>
+        <v>844</v>
       </c>
       <c r="E13" t="s">
-        <v>304</v>
+        <v>846</v>
       </c>
       <c r="F13" t="s">
-        <v>300</v>
+        <v>847</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>845</v>
       </c>
       <c r="I13" t="s">
-        <v>299</v>
+        <v>843</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="B14" t="s">
-        <v>435</v>
+        <v>303</v>
       </c>
       <c r="C14" t="s">
-        <v>436</v>
+        <v>302</v>
       </c>
       <c r="D14" t="s">
-        <v>438</v>
+        <v>301</v>
       </c>
       <c r="E14" t="s">
         <v>304</v>
       </c>
       <c r="F14" t="s">
-        <v>437</v>
+        <v>300</v>
       </c>
       <c r="G14" t="s">
-        <v>439</v>
+        <v>63</v>
       </c>
       <c r="I14" t="s">
-        <v>436</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B15" t="s">
         <v>435</v>
       </c>
       <c r="C15" t="s">
-        <v>1338</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>1339</v>
+        <v>436</v>
+      </c>
+      <c r="D15" t="s">
+        <v>438</v>
       </c>
       <c r="E15" t="s">
-        <v>846</v>
+        <v>304</v>
       </c>
       <c r="F15" t="s">
-        <v>1341</v>
+        <v>437</v>
       </c>
       <c r="G15" t="s">
-        <v>1340</v>
+        <v>439</v>
       </c>
       <c r="I15" t="s">
-        <v>1338</v>
+        <v>436</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="B16" t="s">
-        <v>931</v>
+        <v>435</v>
       </c>
       <c r="C16" t="s">
-        <v>932</v>
-      </c>
-      <c r="D16" t="s">
-        <v>933</v>
+        <v>1338</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>1339</v>
       </c>
       <c r="E16" t="s">
         <v>846</v>
       </c>
       <c r="F16" t="s">
-        <v>935</v>
+        <v>1341</v>
       </c>
       <c r="G16" t="s">
-        <v>937</v>
+        <v>1340</v>
       </c>
       <c r="I16" t="s">
-        <v>932</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="B17" t="s">
         <v>931</v>
       </c>
       <c r="C17" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="D17" t="s">
-        <v>963</v>
+        <v>933</v>
       </c>
       <c r="E17" t="s">
         <v>846</v>
       </c>
       <c r="F17" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="G17" t="s">
         <v>937</v>
       </c>
       <c r="I17" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>459</v>
+        <v>1659</v>
       </c>
       <c r="B18" t="s">
-        <v>455</v>
+        <v>931</v>
       </c>
       <c r="C18" t="s">
-        <v>458</v>
+        <v>934</v>
       </c>
       <c r="D18" t="s">
-        <v>456</v>
+        <v>963</v>
       </c>
       <c r="E18" t="s">
-        <v>457</v>
+        <v>846</v>
       </c>
       <c r="F18" t="s">
-        <v>458</v>
+        <v>936</v>
       </c>
       <c r="G18" t="s">
-        <v>460</v>
+        <v>937</v>
       </c>
       <c r="I18" t="s">
-        <v>458</v>
+        <v>934</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>564</v>
+        <v>459</v>
       </c>
       <c r="B19" t="s">
         <v>455</v>
       </c>
       <c r="C19" t="s">
-        <v>561</v>
+        <v>458</v>
       </c>
       <c r="D19" t="s">
-        <v>563</v>
+        <v>456</v>
       </c>
       <c r="E19" t="s">
-        <v>562</v>
+        <v>457</v>
       </c>
       <c r="F19" t="s">
-        <v>561</v>
+        <v>458</v>
       </c>
       <c r="G19" t="s">
-        <v>560</v>
+        <v>460</v>
       </c>
       <c r="I19" t="s">
-        <v>561</v>
+        <v>458</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B20" t="s">
         <v>455</v>
       </c>
       <c r="C20" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="D20" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E20" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="F20" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="G20" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="I20" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>728</v>
+        <v>568</v>
       </c>
       <c r="B21" t="s">
         <v>455</v>
       </c>
       <c r="C21" t="s">
-        <v>729</v>
+        <v>565</v>
       </c>
       <c r="D21" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="E21" t="s">
-        <v>730</v>
+        <v>567</v>
       </c>
       <c r="F21" t="s">
-        <v>729</v>
+        <v>565</v>
       </c>
       <c r="G21" t="s">
-        <v>734</v>
+        <v>565</v>
       </c>
       <c r="I21" t="s">
-        <v>729</v>
+        <v>565</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="B22" t="s">
         <v>455</v>
       </c>
       <c r="C22" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="D22" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E22" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="F22" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="G22" t="s">
-        <v>565</v>
+        <v>734</v>
       </c>
       <c r="I22" t="s">
-        <v>565</v>
+        <v>729</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="B23" t="s">
         <v>455</v>
       </c>
       <c r="C23" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="D23" t="s">
-        <v>737</v>
+        <v>566</v>
       </c>
       <c r="E23" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="F23" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="G23" t="s">
-        <v>736</v>
+        <v>565</v>
       </c>
       <c r="I23" t="s">
-        <v>736</v>
+        <v>565</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="B24" t="s">
         <v>455</v>
       </c>
       <c r="C24" t="s">
-        <v>739</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>741</v>
+        <v>736</v>
+      </c>
+      <c r="D24" t="s">
+        <v>737</v>
       </c>
       <c r="E24" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="F24" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="G24" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="I24" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>915</v>
+        <v>740</v>
       </c>
       <c r="B25" t="s">
         <v>455</v>
       </c>
       <c r="C25" t="s">
-        <v>916</v>
-      </c>
-      <c r="D25" t="s">
-        <v>917</v>
+        <v>739</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>741</v>
       </c>
       <c r="E25" t="s">
-        <v>918</v>
+        <v>742</v>
       </c>
       <c r="F25" t="s">
-        <v>916</v>
+        <v>739</v>
       </c>
       <c r="G25" t="s">
-        <v>916</v>
+        <v>739</v>
       </c>
       <c r="I25" t="s">
-        <v>916</v>
+        <v>739</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="B26" t="s">
+        <v>455</v>
+      </c>
+      <c r="C26" t="s">
+        <v>916</v>
+      </c>
+      <c r="D26" t="s">
+        <v>917</v>
+      </c>
+      <c r="E26" t="s">
+        <v>918</v>
+      </c>
+      <c r="F26" t="s">
+        <v>916</v>
+      </c>
+      <c r="G26" t="s">
+        <v>916</v>
+      </c>
+      <c r="I26" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>1660</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>1273</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>1275</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>1277</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>1276</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>1275</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>1274</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I27" t="s">
         <v>1278</v>
       </c>
     </row>
@@ -13513,10 +13720,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C302E28E-61B5-45F2-9EED-9E658F066E8B}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13529,7 +13736,7 @@
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13922,6 +14129,84 @@
       </c>
       <c r="I14" t="s">
         <v>1479</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1751</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1752</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1745</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>1749</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1745</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1753</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1748</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>1750</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1748</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1753</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1747</v>
       </c>
     </row>
   </sheetData>
@@ -15791,7 +16076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC079E-4192-4042-9084-101DC20DC760}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -16746,11 +17031,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F28B83C-EC15-4DE5-B23D-95C2173BD368}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -16825,51 +17110,51 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>1502</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>1501</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
-        <v>1499</v>
+        <v>114</v>
       </c>
       <c r="E3" t="s">
         <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>1500</v>
+        <v>116</v>
       </c>
       <c r="G3" t="s">
-        <v>1503</v>
+        <v>115</v>
       </c>
       <c r="I3" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>1566</v>
+        <v>1502</v>
       </c>
       <c r="B4" t="s">
         <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>1567</v>
+        <v>1501</v>
       </c>
       <c r="D4" t="s">
-        <v>1568</v>
+        <v>1499</v>
       </c>
       <c r="E4" t="s">
-        <v>1569</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>1567</v>
+        <v>1500</v>
       </c>
       <c r="G4" t="s">
-        <v>85</v>
+        <v>1503</v>
       </c>
       <c r="I4" t="s">
         <v>89</v>
@@ -16877,28 +17162,28 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>119</v>
+        <v>1566</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>1567</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>1568</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>1569</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>1567</v>
       </c>
       <c r="G5" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="I5" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -17270,77 +17555,77 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>1715</v>
+        <v>216</v>
       </c>
       <c r="B20" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C20" t="s">
-        <v>1716</v>
+        <v>214</v>
       </c>
       <c r="D20" t="s">
-        <v>1719</v>
+        <v>603</v>
       </c>
       <c r="E20" t="s">
-        <v>1717</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>1716</v>
+        <v>215</v>
       </c>
       <c r="G20" t="s">
-        <v>1424</v>
+        <v>217</v>
       </c>
       <c r="I20" t="s">
-        <v>1718</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>216</v>
+        <v>601</v>
       </c>
       <c r="B21" t="s">
         <v>213</v>
       </c>
       <c r="C21" t="s">
-        <v>214</v>
+        <v>602</v>
       </c>
       <c r="D21" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="E21" t="s">
         <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>215</v>
+        <v>605</v>
       </c>
       <c r="G21" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="I21" t="s">
-        <v>218</v>
+        <v>606</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>601</v>
+        <v>772</v>
       </c>
       <c r="B22" t="s">
         <v>213</v>
       </c>
       <c r="C22" t="s">
-        <v>602</v>
+        <v>773</v>
       </c>
       <c r="D22" t="s">
-        <v>604</v>
+        <v>774</v>
       </c>
       <c r="E22" t="s">
         <v>56</v>
       </c>
       <c r="F22" t="s">
-        <v>605</v>
+        <v>775</v>
       </c>
       <c r="G22" t="s">
-        <v>210</v>
+        <v>767</v>
       </c>
       <c r="I22" t="s">
         <v>606</v>
@@ -17348,25 +17633,25 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>772</v>
+        <v>848</v>
       </c>
       <c r="B23" t="s">
         <v>213</v>
       </c>
       <c r="C23" t="s">
-        <v>773</v>
+        <v>849</v>
       </c>
       <c r="D23" t="s">
-        <v>774</v>
+        <v>850</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>769</v>
       </c>
       <c r="F23" t="s">
-        <v>775</v>
+        <v>849</v>
       </c>
       <c r="G23" t="s">
-        <v>767</v>
+        <v>851</v>
       </c>
       <c r="I23" t="s">
         <v>606</v>
@@ -17374,54 +17659,54 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c r="B24" t="s">
         <v>213</v>
       </c>
       <c r="C24" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="D24" t="s">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c r="E24" t="s">
-        <v>769</v>
+        <v>855</v>
       </c>
       <c r="F24" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="G24" t="s">
-        <v>851</v>
+        <v>856</v>
       </c>
       <c r="I24" t="s">
-        <v>606</v>
+        <v>853</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>852</v>
+        <v>1062</v>
       </c>
       <c r="B25" t="s">
-        <v>213</v>
+        <v>1061</v>
       </c>
       <c r="C25" t="s">
-        <v>853</v>
+        <v>1065</v>
       </c>
       <c r="D25" t="s">
-        <v>854</v>
+        <v>1067</v>
       </c>
       <c r="E25" t="s">
-        <v>855</v>
+        <v>1064</v>
       </c>
       <c r="F25" t="s">
-        <v>853</v>
+        <v>1063</v>
       </c>
       <c r="G25" t="s">
-        <v>856</v>
+        <v>1066</v>
       </c>
       <c r="I25" t="s">
-        <v>853</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -17452,33 +17737,59 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>1062</v>
+        <v>1715</v>
       </c>
       <c r="B27" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1716</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1719</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1716</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1424</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B28" t="s">
         <v>1061</v>
       </c>
-      <c r="C27" t="s">
-        <v>1065</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C28" t="s">
+        <v>1737</v>
+      </c>
+      <c r="D28" t="s">
         <v>1067</v>
       </c>
-      <c r="E27" t="s">
-        <v>1064</v>
-      </c>
-      <c r="F27" t="s">
-        <v>1063</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="E28" t="s">
+        <v>1736</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1737</v>
+      </c>
+      <c r="G28" t="s">
         <v>1066</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I28" t="s">
         <v>1063</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{8F28B83C-EC15-4DE5-B23D-95C2173BD368}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J17">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J28">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
add EFMic and ACX
</commit_message>
<xml_diff>
--- a/WyyComponentDatabase.xlsx
+++ b/WyyComponentDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cadence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56D7274-8F03-4764-8C9C-FD1438232498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FE18D9-7E6B-48A1-864D-45C6FF515CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15450" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3171" uniqueCount="1775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3205" uniqueCount="1801">
   <si>
     <t>Part Number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6913,6 +6913,106 @@
   </si>
   <si>
     <t>bga153_13rx11r5</t>
+  </si>
+  <si>
+    <t>射频功放</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2083100000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2083100001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QPF4206B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qorvo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qfn16_3x3_FEM</t>
+  </si>
+  <si>
+    <t>qfn16_3x3_FEM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKY85337-11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKY85755-11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QPF4526</t>
+  </si>
+  <si>
+    <t>QPF4526TR13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QPF4206BTR13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">QPF4206BTR13; 33 dB Tx Gain; 1.9 dB Noise Figure; 14.5 dB Rx Gain &amp; 8 dB Bypass Loss; 25 dB 2.4 GHz Rejection on Rx Path </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2412 – 2484 MHz; 33 dB Tx Gain; 2.1 dB Noise Figure; 15 dB Rx Gain &amp; 6 dB Bypass Loss; 25 dB 5 GHz Rejection on Rx Path; </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3x3mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC耦合器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2083200000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2083200001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CP0605-19D2455AB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CP0605-18V6140AM</t>
+  </si>
+  <si>
+    <t>DPLX-DP2012-E2455BA-ACX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>couplers_4p_smd_cp0605</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACX(璟德)</t>
+  </si>
+  <si>
+    <t>(2400 ~ 2500 Insertion Loss: 0.2 max.@-40~85℃ 0.25 max.@105℃)(4900 ~ 5950 Insertion Loss: 0.5 max.@-40~85℃ 0.55 max.@105℃)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CP0605-18V6140AM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(5150 ~ 6140 &amp; 6140 ~ 7125 Insertion Loss: 0.5 max.(25°C) 0.9 max.(-40 to 100°C))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -11970,10 +12070,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC4AD67-C776-4093-88E2-79BBC414D956}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11981,11 +12081,11 @@
     <col min="1" max="1" width="11.875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="101.5" customWidth="1"/>
+    <col min="4" max="4" width="118" customWidth="1"/>
     <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -12720,6 +12820,116 @@
       </c>
       <c r="I28" t="s">
         <v>1275</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1775</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1778</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1788</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1779</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1786</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1781</v>
+      </c>
+      <c r="H29" t="s">
+        <v>1789</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1775</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1784</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1787</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1779</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1785</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1780</v>
+      </c>
+      <c r="H30" t="s">
+        <v>1789</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1790</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1793</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>1798</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1793</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1796</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1790</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1799</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1800</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1794</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1796</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>